<commit_message>
now improvided code for accessing methods using playwright capabilities
</commit_message>
<xml_diff>
--- a/testData/amazonSteps - Copy (2).xlsx
+++ b/testData/amazonSteps - Copy (2).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/ZS_Playwright_GenAI/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2256D388-8D4E-492D-A4EC-77AAE3896D62}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBC2029C-8C67-48CE-883F-F44B248C00CD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
   <si>
     <t>action</t>
   </si>
@@ -49,61 +49,103 @@
     <t>https://www.amazon.com/</t>
   </si>
   <si>
+    <t>Hello, Sign in</t>
+  </si>
+  <si>
+    <t>weavernormar@gmail.com</t>
+  </si>
+  <si>
+    <t>Welcome@123456</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/cart/view.html?ref_=nav_cart</t>
+  </si>
+  <si>
+    <t>assert</t>
+  </si>
+  <si>
+    <t>h2#deliver-to-customer-text</t>
+  </si>
+  <si>
+    <t>Delivering to Normar Weaver</t>
+  </si>
+  <si>
+    <t>waitfortext</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>#subtotals-marketplace-table</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>TestID</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>locatorType</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>span</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Sign in</t>
+  </si>
+  <si>
+    <t>Search Amazon</t>
+  </si>
+  <si>
+    <t>Go</t>
+  </si>
+  <si>
+    <t>Proceed to checkout</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>SAMSUNG 85-Inch Class Crystal UHD 4K DU7200 Series HDR Smart TV w/Object Tracking Sound Lite, PurColor, Motion Xcelerator, Mega Contrast, Q-Symphony (UN85DU7200, 2024 Model)</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
     <t>type</t>
   </si>
   <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>Hello, Sign in</t>
-  </si>
-  <si>
-    <t>email input field</t>
-  </si>
-  <si>
-    <t>weavernormar@gmail.com</t>
-  </si>
-  <si>
-    <t>Continue button on page</t>
-  </si>
-  <si>
-    <t>password input field in span</t>
-  </si>
-  <si>
-    <t>Welcome@123456</t>
-  </si>
-  <si>
-    <t>signin button on page</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/gp/cart/view.html?ref_=nav_cart</t>
-  </si>
-  <si>
-    <t>assert</t>
-  </si>
-  <si>
-    <t>h2#deliver-to-customer-text</t>
-  </si>
-  <si>
-    <t>Delivering to Normar Weaver</t>
-  </si>
-  <si>
-    <t>waitfortext</t>
-  </si>
-  <si>
-    <t>Continue</t>
-  </si>
-  <si>
-    <t>clickloc</t>
-  </si>
-  <si>
-    <t>input[name="proceedToRetailCheckout"]</t>
-  </si>
-  <si>
-    <t>#subtotals-marketplace-table</t>
-  </si>
-  <si>
-    <t>Automation</t>
+    <t>scroll</t>
+  </si>
+  <si>
+    <t>Add to cart</t>
+  </si>
+  <si>
+    <t>button</t>
   </si>
 </sst>
 </file>
@@ -448,207 +490,432 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:H18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="73.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="36" style="1" customWidth="1"/>
+    <col min="4" max="4" width="51.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="G2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="G8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H8" s="1">
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H9" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E15" s="2"/>
+      <c r="G15" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H15" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H16" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H17" s="1">
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E10" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E11" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E12" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="G18" s="1">
         <v>1000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{BA0E224C-C858-47AF-8859-A659DB8B5C6D}"/>
-    <hyperlink ref="C8" r:id="rId2" xr:uid="{AB3D6231-B488-4B94-BF6C-F9D8D7D5C450}"/>
-    <hyperlink ref="B10" r:id="rId3" xr:uid="{49C1B01C-0762-43C0-9564-0E997C4E221F}"/>
+    <hyperlink ref="F6" r:id="rId1" xr:uid="{BA0E224C-C858-47AF-8859-A659DB8B5C6D}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{AB3D6231-B488-4B94-BF6C-F9D8D7D5C450}"/>
+    <hyperlink ref="D15" r:id="rId3" xr:uid="{49C1B01C-0762-43C0-9564-0E997C4E221F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
new changes for poc
</commit_message>
<xml_diff>
--- a/testData/amazonSteps - Copy (2).xlsx
+++ b/testData/amazonSteps - Copy (2).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/ZS_Playwright_GenAI/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/QATaskAutomation/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="182" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBC2029C-8C67-48CE-883F-F44B248C00CD}"/>
@@ -492,9 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:H18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>